<commit_message>
Atualização do arquivo após o brainstorm
</commit_message>
<xml_diff>
--- a/PastaDocumentos/2SIPH-ListaRequisitos-SiEstacionamento.xlsx
+++ b/PastaDocumentos/2SIPH-ListaRequisitos-SiEstacionamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIAP-2024\TEMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37333D0C-DA00-4863-B846-A6DEB4D0481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F45244-D960-432F-8BE7-BB261E2572E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{42041E6B-20B5-40F2-9291-CD50E6A1A57E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Lista de requisitos</t>
   </si>
@@ -100,6 +100,90 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Terminal mobile de atendimento;</t>
+  </si>
+  <si>
+    <t>Sensor de vagas livres/ocupadas</t>
+  </si>
+  <si>
+    <t>Controle de filas de entrada e saída</t>
+  </si>
+  <si>
+    <t>Controle de tickets</t>
+  </si>
+  <si>
+    <t>Tratamento de meios de pagamento</t>
+  </si>
+  <si>
+    <t>Tipificação de uso (mensalista/avulso/conveniado)</t>
+  </si>
+  <si>
+    <t>Administração de caixa</t>
+  </si>
+  <si>
+    <t>Configuração de tabelas preços (dias/horários/tipo de uso)</t>
+  </si>
+  <si>
+    <t>Emissão de nota fiscal</t>
+  </si>
+  <si>
+    <t>Gestão de cobranças de mensalistas e conveniados</t>
+  </si>
+  <si>
+    <t>Reconhecimento de placa para recuperar dados cadastrais</t>
+  </si>
+  <si>
+    <t>Cadastro de veículos e clientes</t>
+  </si>
+  <si>
+    <t>Reservar vagas</t>
+  </si>
+  <si>
+    <t>Solução mobile para o cliente fazer reservas e pagamentos</t>
+  </si>
+  <si>
+    <t>Orientação por voz</t>
+  </si>
+  <si>
+    <t>Integração com TAG</t>
+  </si>
+  <si>
+    <t>Relatório de gerenciamento de média de ocupação de vagas por dia e horário</t>
+  </si>
+  <si>
+    <t>Relatório de gerenciamento do valor recebido por meio de pagamento por mês</t>
+  </si>
+  <si>
+    <t>Forum/Sistema de Denuncias</t>
+  </si>
+  <si>
+    <t>Estacionamento Vertical com elevador</t>
+  </si>
+  <si>
+    <t>Planta digital</t>
+  </si>
+  <si>
+    <t>Sistema de fidelidade</t>
+  </si>
+  <si>
+    <t>Controle do período estacionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema de vigilância automatizado, com câmeras inteligentes. </t>
+  </si>
+  <si>
+    <t>Ticket digital via e-mail ou sms</t>
+  </si>
+  <si>
+    <t>Sistema de Segurança contra roubos </t>
+  </si>
+  <si>
+    <t>Sistema de redirecionamento para o condutor indicando vagas livres</t>
+  </si>
+  <si>
+    <t>Mostrar quantidade de vagas disponíveis em determinado local</t>
   </si>
 </sst>
 </file>
@@ -202,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -226,9 +310,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,19 +624,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2924E7E3-4BB6-4F36-B430-910D22753DB0}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.85546875" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="92.28515625" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,101 +792,256 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="10"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="15"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1017,9 +1253,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE55239-3B84-4C7D-85A8-1299C75BC4A3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94B110F6-A58A-401B-8264-725C7B4C4EED}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9836474-5EE6-4417-B4D0-222B651917AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B232DBC-6394-4A73-90FA-9B739EBD8139}"/>
 </file>
</xml_diff>